<commit_message>
functional tests for offer making (part 3 - database test the offer went through)
</commit_message>
<xml_diff>
--- a/proj_aged/core/aged/lab/DataSafeOnes/17_just_two_sales_people.xlsx
+++ b/proj_aged/core/aged/lab/DataSafeOnes/17_just_two_sales_people.xlsx
@@ -1298,11 +1298,11 @@
   </sheetPr>
   <dimension ref="B1:E375"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A313" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D329" activeCellId="0" sqref="D329"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A145" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B160" activeCellId="0" sqref="B160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.40625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.41796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>

</xml_diff>